<commit_message>
turns out what I thought was a bug with SLIDE_WIN_CENTER option was actually a bug with the UL CNR option.  Unfortunately the correct GAIN_AND_OFFSET model does not provide good results as the gain sometimes goes -ve.
</commit_message>
<xml_diff>
--- a/Docs/Funding/GEF5/GEF5 SLM BUDGET REQUEST SHEET.xlsx
+++ b/Docs/Funding/GEF5/GEF5 SLM BUDGET REQUEST SHEET.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\Projects\PhD GeoInformatics\Docs\Funding\GEF5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -35,12 +40,12 @@
     <definedName name="wwf_daily_indirect">[1]Assumptions!$B$19</definedName>
     <definedName name="WWF_rate">[1]Assumptions!$B$12</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>3.1a</t>
   </si>
@@ -48,15 +53,9 @@
     <t>Comprehensive literature review of methodologies for CDM and VCS restoration projects conducted by local consultant.</t>
   </si>
   <si>
-    <t>Local consultant to devise methodology from remote sensing analyses and baseline field sampling, starting in YR1 and continuing into YR2 and 3.</t>
-  </si>
-  <si>
     <t>3.1d</t>
   </si>
   <si>
-    <t>Engagement to begin in YR1 and continue into yr 5 (will need to extend beyond the methodology development to ensure uptake in phase 2 of carbon tax)</t>
-  </si>
-  <si>
     <t>Report summarizing outcomes of government engagement activities conducted in YR1 and implications for getting new methodology approved.</t>
   </si>
   <si>
@@ -90,27 +89,12 @@
     <t>1) Progress report on literature review for carbon methodologies.                                                                                                    2) A literature review of CDM and VCS  methodologies for restoration projects with discussion of the implications for applying to local context (Baviaans)</t>
   </si>
   <si>
-    <t>2 weeks WWF time (@ xx ZAR/month); 1 trip field trip (@ xx ZAR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consultant fees for time at xx hours or days at xx ZAR/hr or ZAR/day                                                                                                          Travel expenses at xx ZAR for 10 day field trip                                   Subsistence at xx ZAR for 10 day field trip                                                     Equipment at xx ZAR for 10 raintainks.                                         </t>
-  </si>
-  <si>
     <t>OUTPUT CODE</t>
   </si>
   <si>
-    <t xml:space="preserve">1) Report detailing progress toward devising a carbon methodology using remote sensing and field baselines.  </t>
-  </si>
-  <si>
-    <t>2 months consultant time at ZAR 400/hr for 40 days work</t>
-  </si>
-  <si>
     <t>Q2</t>
   </si>
   <si>
-    <t>WWF/LL/Cosman Bolus/Dugal Harris</t>
-  </si>
-  <si>
     <t>Q4 (Oct-Dec)</t>
   </si>
   <si>
@@ -121,6 +105,21 @@
   </si>
   <si>
     <t xml:space="preserve">ORGANIZATION/PERSON </t>
+  </si>
+  <si>
+    <t>Dugal Harris</t>
+  </si>
+  <si>
+    <t>3 months consultant time at ZAR 300/hr for 12 days work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Apply differential correction to field DGPS data acquired during Q1&amp;2.
+2) Process Q1&amp;2 field allometric data to produce woody carbon stock (CS) estimates.
+3) Perform preliminary correlation analysis on data acquired to date. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Results of activ ities 1-3 (models, graphs and correlation statistics).  </t>
   </si>
 </sst>
 </file>
@@ -128,11 +127,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="[$$-409]#,##0"/>
-    <numFmt numFmtId="167" formatCode="&quot;R&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="[$$-409]#,##0"/>
+    <numFmt numFmtId="168" formatCode="&quot;R&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -382,21 +381,21 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -430,35 +429,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -467,26 +460,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="168" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -514,10 +501,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -530,6 +517,21 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -545,6 +547,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -715,7 +785,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="B9B9B9"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -750,7 +820,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -785,7 +855,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1002,7 +1072,7 @@
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1019,10 +1089,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="34"/>
+      <c r="A1" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="47"/>
       <c r="C1" s="3"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -1038,8 +1108,8 @@
       <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:28" s="10" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1055,18 +1125,18 @@
       <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="35">
+      <c r="A3" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="31">
         <v>2018</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="18"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1077,14 +1147,14 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="17"/>
+      <c r="S3" s="16"/>
     </row>
     <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>21</v>
+      <c r="A4" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2"/>
@@ -1101,18 +1171,18 @@
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:28" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="20"/>
+      <c r="A5" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -1123,17 +1193,17 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="17"/>
+      <c r="S5" s="16"/>
     </row>
     <row r="6" spans="1:28" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="20"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -1144,32 +1214,32 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="17"/>
+      <c r="S6" s="16"/>
     </row>
     <row r="7" spans="1:28" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="23" t="s">
+      <c r="A7" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="21" t="s">
         <v>10</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>12</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -1177,27 +1247,20 @@
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:28" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="28">
-        <f>2237*13</f>
-        <v>29081</v>
-      </c>
-      <c r="E8" s="29">
-        <v>30000</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="26" t="s">
-        <v>17</v>
-      </c>
+      <c r="C8" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="14"/>
       <c r="J8" s="11"/>
       <c r="K8" s="12"/>
@@ -1208,43 +1271,43 @@
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="48"/>
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
       <c r="AA8" s="14"/>
       <c r="AB8" s="12"/>
     </row>
-    <row r="9" spans="1:28" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="28">
+    <row r="9" spans="1:28" s="15" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="26">
         <v>25200</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="27">
         <v>25200</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="26">
         <v>63000</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="28">
         <v>78094.5</v>
       </c>
-      <c r="H9" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="22"/>
+      <c r="H9" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="20"/>
       <c r="J9" s="11"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -1266,26 +1329,18 @@
       <c r="AB9" s="12"/>
     </row>
     <row r="10" spans="1:28" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="44">
-        <v>1618.2592592592594</v>
-      </c>
-      <c r="E10" s="45">
-        <v>20000</v>
-      </c>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="46" t="s">
-        <v>16</v>
-      </c>
+      <c r="D10" s="40"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="42"/>
       <c r="I10" s="14"/>
       <c r="J10" s="11"/>
       <c r="K10" s="12"/>
@@ -1299,37 +1354,37 @@
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
       <c r="AA10" s="14"/>
       <c r="AB10" s="12"/>
     </row>
     <row r="11" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="47"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="33">
+      <c r="A11" s="43"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="30">
         <f>SUM(D8:D10)</f>
-        <v>55899.259259259263</v>
-      </c>
-      <c r="E11" s="32">
+        <v>25200</v>
+      </c>
+      <c r="E11" s="29">
         <f t="shared" ref="E11:G11" si="0">SUM(E8:E10)</f>
-        <v>75200</v>
-      </c>
-      <c r="F11" s="33">
+        <v>25200</v>
+      </c>
+      <c r="F11" s="30">
         <f t="shared" si="0"/>
         <v>63000</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="30">
         <f t="shared" si="0"/>
         <v>78094.5</v>
       </c>
-      <c r="H11" s="50"/>
+      <c r="H11" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>